<commit_message>
Updated CO configuration.xlsx with additional skillsets
git-svn-id: svn://svn-staging.maximus.com/dev1d/maxdat@12025 3a208796-2f9a-46b6-afea-cdc47f3b9e6b
</commit_message>
<xml_diff>
--- a/ContactCenter/trunk/kettle/MAXDAT/implementation/CO/data/configuration.xlsx
+++ b/ContactCenter/trunk/kettle/MAXDAT/implementation/CO/data/configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="11280" windowHeight="7725" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="11280" windowHeight="7725" tabRatio="762" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="297">
   <si>
     <t>PROJECT_NAME</t>
   </si>
@@ -1157,6 +1157,45 @@
   </si>
   <si>
     <t>DUMMY</t>
+  </si>
+  <si>
+    <t>Default ACD</t>
+  </si>
+  <si>
+    <t>Default_Skillset</t>
+  </si>
+  <si>
+    <t>IEVS_Eng_sk</t>
+  </si>
+  <si>
+    <t>Pk_BIWAD_SP_sk</t>
+  </si>
+  <si>
+    <t>AAB_SP_sk</t>
+  </si>
+  <si>
+    <t>OMB_eng_sk</t>
+  </si>
+  <si>
+    <t>OMB_spn_sk</t>
+  </si>
+  <si>
+    <t>FML_eng_sk</t>
+  </si>
+  <si>
+    <t>FML_spn_sk</t>
+  </si>
+  <si>
+    <t>CHP_eng_sk</t>
+  </si>
+  <si>
+    <t>CHP_spn_sk</t>
+  </si>
+  <si>
+    <t>PAC_Eng_sk</t>
+  </si>
+  <si>
+    <t>PAC_Spn_sk</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1312,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1295,7 +1334,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1683,7 +1721,7 @@
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>281</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -1937,7 +1975,7 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1964,31 +2002,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -2019,50 +2057,50 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+    <row r="2" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
         <v>10000</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="23">
+      <c r="C2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="22">
         <v>0</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <v>30</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="22">
         <v>15</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="M2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="23" t="s">
+      <c r="M2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>33</v>
       </c>
       <c r="P2" s="15">
@@ -2071,54 +2109,54 @@
       <c r="Q2" s="15">
         <v>401768</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="22" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+    <row r="3" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
         <v>10001</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="23">
+      <c r="C3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="22">
         <v>0</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>30</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>15</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="M3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="23" t="s">
+      <c r="M3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="P3" s="15">
@@ -2127,7 +2165,7 @@
       <c r="Q3" s="15">
         <v>401768</v>
       </c>
-      <c r="R3" s="23" t="s">
+      <c r="R3" s="22" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2138,34 +2176,34 @@
       <c r="B4" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="19">
         <v>0</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>30</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <v>15</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M4" s="11" t="s">
@@ -2194,34 +2232,34 @@
       <c r="B5" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="19">
         <v>0</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>30</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <v>15</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M5" s="11" t="s">
@@ -2250,34 +2288,34 @@
       <c r="B6" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="19">
         <v>0</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>30</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="22">
         <v>15</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M6" s="11" t="s">
@@ -2306,34 +2344,34 @@
       <c r="B7" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="19">
         <v>0</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>30</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="22">
         <v>15</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M7" s="11" t="s">
@@ -2355,50 +2393,50 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+    <row r="8" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
         <v>10014</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="23">
+      <c r="C8" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="22">
         <v>0</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>30</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>15</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="M8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="23" t="s">
+      <c r="M8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="22" t="s">
         <v>33</v>
       </c>
       <c r="P8" s="15">
@@ -2407,7 +2445,7 @@
       <c r="Q8" s="15">
         <v>401768</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="R8" s="22" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2418,34 +2456,34 @@
       <c r="B9" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="19">
         <v>0</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <v>30</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="22">
         <v>15</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L9" s="23" t="s">
+      <c r="L9" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M9" s="11" t="s">
@@ -2474,34 +2512,34 @@
       <c r="B10" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="19">
         <v>0</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>30</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="22">
         <v>15</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="L10" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M10" s="11" t="s">
@@ -2530,34 +2568,34 @@
       <c r="B11" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="19">
         <v>0</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <v>30</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="22">
         <v>15</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="L11" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M11" s="11" t="s">
@@ -2586,34 +2624,34 @@
       <c r="B12" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="19">
         <v>0</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <v>30</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="22">
         <v>15</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M12" s="11" t="s">
@@ -2642,34 +2680,34 @@
       <c r="B13" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="19">
         <v>0</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <v>30</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="22">
         <v>15</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M13" s="11" t="s">
@@ -2698,34 +2736,34 @@
       <c r="B14" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="19">
         <v>0</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <v>30</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="22">
         <v>15</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="K14" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="L14" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M14" s="11" t="s">
@@ -2754,34 +2792,34 @@
       <c r="B15" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="19">
         <v>0</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="22">
         <v>30</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="22">
         <v>15</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M15" s="11" t="s">
@@ -2810,34 +2848,34 @@
       <c r="B16" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="19">
         <v>0</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <v>30</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="22">
         <v>15</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="L16" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M16" s="11" t="s">
@@ -2866,34 +2904,34 @@
       <c r="B17" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="19">
         <v>0</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <v>30</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="22">
         <v>15</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="H17" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M17" s="11" t="s">
@@ -2922,34 +2960,34 @@
       <c r="B18" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="19">
         <v>0</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>30</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="22">
         <v>15</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M18" s="20" t="s">
@@ -2978,34 +3016,34 @@
       <c r="B19" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="19">
         <v>0</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <v>30</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="22">
         <v>15</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M19" s="20" t="s">
@@ -3034,34 +3072,34 @@
       <c r="B20" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="19">
         <v>0</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <v>30</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="22">
         <v>15</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J20" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="K20" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L20" s="23" t="s">
+      <c r="L20" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M20" s="20" t="s">
@@ -3090,34 +3128,34 @@
       <c r="B21" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="19">
         <v>0</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="22">
         <v>30</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="22">
         <v>15</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="I21" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K21" s="23" t="s">
+      <c r="K21" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L21" s="23" t="s">
+      <c r="L21" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M21" s="20" t="s">
@@ -3146,34 +3184,34 @@
       <c r="B22" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="19">
         <v>0</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="22">
         <v>30</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="22">
         <v>15</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K22" s="23" t="s">
+      <c r="K22" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L22" s="23" t="s">
+      <c r="L22" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M22" s="20" t="s">
@@ -3202,34 +3240,34 @@
       <c r="B23" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="19">
         <v>0</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="22">
         <v>30</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="22">
         <v>15</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I23" s="23" t="s">
+      <c r="I23" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J23" s="23" t="s">
+      <c r="J23" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K23" s="23" t="s">
+      <c r="K23" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L23" s="23" t="s">
+      <c r="L23" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M23" s="20" t="s">
@@ -3258,34 +3296,34 @@
       <c r="B24" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="19">
         <v>0</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="22">
         <v>30</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="22">
         <v>15</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K24" s="23" t="s">
+      <c r="K24" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M24" s="20" t="s">
@@ -3314,34 +3352,34 @@
       <c r="B25" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="19">
         <v>0</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="22">
         <v>30</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="22">
         <v>15</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="G25" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="I25" s="23" t="s">
+      <c r="I25" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="J25" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="K25" s="23" t="s">
+      <c r="K25" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="L25" s="23" t="s">
+      <c r="L25" s="22" t="s">
         <v>237</v>
       </c>
       <c r="M25" s="20" t="s">
@@ -3363,16 +3401,16 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="29"/>
-    </row>
-    <row r="27" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="28"/>
+    </row>
+    <row r="27" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="22" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A2:R28">
     <sortCondition descending="1" sortBy="cellColor" ref="B2:B28" dxfId="0"/>
@@ -3388,10 +3426,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,603 +3466,695 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+    <row r="2" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28">
+        <v>2</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>10000</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
         <v>10002</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B4" s="28" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C4" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D4" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E4" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F4" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G4" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
         <v>10003</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B5" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C5" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D5" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E5" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F5" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G5" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+    <row r="6" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
         <v>10004</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B6" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C6" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D6" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E6" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F6" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G6" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+    <row r="7" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
         <v>10020</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B7" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C7" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D7" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E7" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F7" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G7" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+    <row r="8" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
         <v>10021</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B8" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C8" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D8" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E8" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F8" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G8" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+    <row r="9" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
         <v>10022</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B9" s="28" t="s">
         <v>269</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C9" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D9" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E9" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F9" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G9" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+    <row r="10" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
         <v>10023</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B10" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C10" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D10" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E10" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F10" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G10" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+    <row r="11" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
+        <v>10024</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28">
         <v>10025</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B12" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C12" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D12" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E12" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F12" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G12" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+    <row r="13" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28">
+        <v>10027</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28">
         <v>10038</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B14" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C14" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D14" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E14" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F14" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G14" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+    <row r="15" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28">
         <v>10039</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B15" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C15" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D15" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E15" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F15" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G15" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+    <row r="16" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28">
         <v>10040</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B16" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C16" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D16" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E16" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F16" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G16" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+    <row r="17" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28">
         <v>10041</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B17" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C17" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D17" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E17" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F17" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G17" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+    <row r="18" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28">
         <v>10042</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B18" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C18" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D18" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E18" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F18" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G18" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+    <row r="19" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
         <v>10043</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B19" s="28" t="s">
         <v>277</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C19" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D19" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E19" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F19" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G19" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+    <row r="20" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28">
         <v>10044</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B20" s="28" t="s">
         <v>278</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C20" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D20" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E20" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F20" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G20" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+    <row r="21" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28">
+        <v>10045</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28">
         <v>10046</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B22" s="28" t="s">
         <v>279</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C22" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D22" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E22" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F22" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G22" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+    <row r="23" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28">
         <v>10047</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B23" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C23" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D23" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E23" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F23" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G23" s="28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
+    <row r="24" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
+        <v>10048</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28">
+        <v>10049</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28">
+        <v>10050</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28">
+        <v>10051</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28">
+        <v>10052</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28">
+        <v>10053</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28">
+        <v>10054</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28">
+        <v>10055</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4046,11 +4176,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="26" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="22" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" style="11" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4059,7 +4189,7 @@
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>236</v>
       </c>
       <c r="C1" s="14" t="s">
@@ -4081,26 +4211,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="22">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4141,19 +4271,19 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -4362,980 +4492,980 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="23"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
       <c r="I55" s="15"/>
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="23"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="22"/>
       <c r="I56" s="15"/>
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="23"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
-      <c r="H57" s="23"/>
+      <c r="A57" s="22"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
       <c r="I57" s="15"/>
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
       <c r="I58" s="15"/>
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23"/>
-      <c r="H60" s="23"/>
+      <c r="A60" s="22"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
       <c r="I60" s="15"/>
       <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="23"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="23"/>
+      <c r="A61" s="22"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23"/>
-      <c r="H62" s="23"/>
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
       <c r="I63" s="15"/>
       <c r="J63" s="15"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="23"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
       <c r="I64" s="15"/>
       <c r="J64" s="15"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="23"/>
-      <c r="H65" s="23"/>
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
       <c r="I65" s="15"/>
       <c r="J65" s="15"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="23"/>
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
+      <c r="A66" s="22"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="22"/>
       <c r="I66" s="15"/>
       <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-      <c r="B67" s="23"/>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
+      <c r="A67" s="22"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
       <c r="I67" s="15"/>
       <c r="J67" s="15"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
-      <c r="B68" s="23"/>
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="23"/>
+      <c r="A68" s="22"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="22"/>
       <c r="I68" s="15"/>
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="23"/>
-      <c r="H69" s="23"/>
+      <c r="A69" s="22"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
       <c r="I69" s="15"/>
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
-      <c r="B70" s="23"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="23"/>
-      <c r="H70" s="23"/>
+      <c r="A70" s="22"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
       <c r="I70" s="15"/>
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="23"/>
-      <c r="H71" s="23"/>
+      <c r="A71" s="22"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
       <c r="I71" s="15"/>
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
-      <c r="B72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
-      <c r="H72" s="23"/>
+      <c r="A72" s="22"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
       <c r="I72" s="15"/>
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
-      <c r="B73" s="23"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
       <c r="I73" s="15"/>
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="23"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="23"/>
+      <c r="A74" s="22"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="23"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="23"/>
-      <c r="H75" s="23"/>
+      <c r="A75" s="22"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
       <c r="I75" s="15"/>
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="23"/>
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23"/>
-      <c r="H76" s="23"/>
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
       <c r="I76" s="15"/>
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
-      <c r="B77" s="23"/>
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
-      <c r="E77" s="23"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
-      <c r="H77" s="23"/>
+      <c r="A77" s="22"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-      <c r="B78" s="23"/>
-      <c r="C78" s="23"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
-      <c r="H78" s="23"/>
+      <c r="A78" s="22"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="22"/>
       <c r="I78" s="15"/>
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="23"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23"/>
-      <c r="H79" s="23"/>
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
-      <c r="B80" s="23"/>
-      <c r="C80" s="23"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="23"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="23"/>
-      <c r="H80" s="23"/>
+      <c r="A80" s="22"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
       <c r="I80" s="15"/>
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
-      <c r="H81" s="23"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
       <c r="I81" s="15"/>
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
-      <c r="B82" s="23"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="23"/>
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
       <c r="I82" s="15"/>
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="23"/>
-      <c r="B83" s="23"/>
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
-      <c r="E83" s="23"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="23"/>
-      <c r="H83" s="23"/>
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
       <c r="I83" s="15"/>
       <c r="J83" s="15"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="23"/>
-      <c r="B84" s="23"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="23"/>
-      <c r="E84" s="23"/>
-      <c r="F84" s="23"/>
-      <c r="G84" s="23"/>
-      <c r="H84" s="23"/>
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+      <c r="H84" s="22"/>
       <c r="I84" s="15"/>
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="23"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="23"/>
-      <c r="D85" s="23"/>
-      <c r="E85" s="23"/>
-      <c r="F85" s="23"/>
-      <c r="G85" s="23"/>
-      <c r="H85" s="23"/>
+      <c r="A85" s="22"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
       <c r="I85" s="15"/>
       <c r="J85" s="15"/>
     </row>
@@ -6739,70 +6869,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="22">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="23">
+      <c r="B2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="22">
         <v>0</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>